<commit_message>
inicio de filtrado de base de datos
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Otros ordenadores\Mi portátil\FILES\UNIVERSITY\2022-2\TECNICAS DE ANALISIS ESTADISTICO\TRABAJOS\TRABAJO 2\Riesgo-Credito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C48B9-ACC2-4B49-84FC-0DBCDC8EA14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7442E42E-BB09-4A2C-ABED-105B4D31E5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -979,7 +979,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -990,6 +990,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF244061"/>
         <bgColor rgb="FF244061"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1040,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1056,6 +1062,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1277,8 +1284,8 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1311,7 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C2" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B2,""en"",""es"")"),"El estado proporcionado por el prestatario en la solicitud de préstamo")</f>
         <v>El estado proporcionado por el prestatario en la solicitud de préstamo</v>
       </c>
@@ -1316,7 +1323,7 @@
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="str">
+      <c r="C3" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B3,""en"",""es"")"),"El ingreso anual autoinformado proporcionado por el prestatario durante el registro.")</f>
         <v>El ingreso anual autoinformado proporcionado por el prestatario durante el registro.</v>
       </c>
@@ -1328,7 +1335,7 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="str">
+      <c r="C4" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B4,""en"",""es"")"),"El ingreso anual autoinformado combinado proporcionado por los co-prestatarios durante el registro")</f>
         <v>El ingreso anual autoinformado combinado proporcionado por los co-prestatarios durante el registro</v>
       </c>
@@ -1340,7 +1347,7 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="str">
+      <c r="C5" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B5,""en"",""es"")"),"Indica si el préstamo es una solicitud individual o una solicitud conjunta con dos co-prestatarios")</f>
         <v>Indica si el préstamo es una solicitud individual o una solicitud conjunta con dos co-prestatarios</v>
       </c>
@@ -1376,7 +1383,7 @@
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="str">
+      <c r="C8" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B8,""en"",""es"")"),"El número de más de 30 días de entrega de la delincuencia en el archivo de crédito del prestatario durante los últimos 2 años")</f>
         <v>El número de más de 30 días de entrega de la delincuencia en el archivo de crédito del prestatario durante los últimos 2 años</v>
       </c>
@@ -1388,7 +1395,7 @@
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4" t="str">
+      <c r="C9" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B9,""en"",""es"")"),"Descripción del préstamo proporcionado por el prestatario")</f>
         <v>Descripción del préstamo proporcionado por el prestatario</v>
       </c>
@@ -1424,7 +1431,7 @@
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="str">
+      <c r="C12" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B12,""en"",""es"")"),"El mes se abrió la línea de crédito más temprana del prestatario")</f>
         <v>El mes se abrió la línea de crédito más temprana del prestatario</v>
       </c>
@@ -1436,7 +1443,7 @@
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="str">
+      <c r="C13" s="11" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B13,""en"",""es"")"),"Longitud del empleo en años. Los valores posibles son entre 0 y 10 donde 0 significa menos de un año y 10 significa diez o más años.")</f>
         <v>Longitud del empleo en años. Los valores posibles son entre 0 y 10 donde 0 significa menos de un año y 10 significa diez o más años.</v>
       </c>

</xml_diff>